<commit_message>
Another change to Manifest
Changed StandAlone to StandAlone_FirstRun
</commit_message>
<xml_diff>
--- a/configs/manifest_apps.xlsx
+++ b/configs/manifest_apps.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
   <si>
     <t>CommitID</t>
   </si>
@@ -46,13 +46,16 @@
     <t>2475fa8</t>
   </si>
   <si>
-    <t>StandAlone</t>
-  </si>
-  <si>
     <t>,</t>
   </si>
   <si>
     <t>APINHO-LT</t>
+  </si>
+  <si>
+    <t>a910999</t>
+  </si>
+  <si>
+    <t>StandAlone_FirstRun</t>
   </si>
 </sst>
 </file>
@@ -402,10 +405,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -443,7 +446,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B2" t="s">
         <v>7</v>
@@ -452,16 +455,21 @@
         <v>8</v>
       </c>
       <c r="D2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" t="s">
         <v>10</v>
       </c>
-      <c r="E2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F2" t="s">
-        <v>11</v>
-      </c>
       <c r="G2" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Deleted commits put in manifest_apps
Manifest apps does not need any commits posted to it for the first time it is launched. I deleted any added commits.
</commit_message>
<xml_diff>
--- a/configs/manifest_apps.xlsx
+++ b/configs/manifest_apps.xlsx
@@ -9,12 +9,12 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
   <si>
     <t>CommitID</t>
   </si>
@@ -43,19 +43,13 @@
     <t>Splunk_Operations</t>
   </si>
   <si>
-    <t>2475fa8</t>
-  </si>
-  <si>
     <t>,</t>
   </si>
   <si>
-    <t>APINHO-LT</t>
-  </si>
-  <si>
-    <t>a910999</t>
-  </si>
-  <si>
     <t>StandAlone_FirstRun</t>
+  </si>
+  <si>
+    <t>ip-10-123-10-250</t>
   </si>
 </sst>
 </file>
@@ -408,7 +402,7 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -445,9 +439,7 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>12</v>
-      </c>
+      <c r="A2" s="1"/>
       <c r="B2" t="s">
         <v>7</v>
       </c>
@@ -455,22 +447,20 @@
         <v>8</v>
       </c>
       <c r="D2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E2" t="s">
         <v>11</v>
       </c>
       <c r="F2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>9</v>
-      </c>
+      <c r="A3" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>